<commit_message>
changes in API and login
</commit_message>
<xml_diff>
--- a/_project-files/estimates.xlsx
+++ b/_project-files/estimates.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1380" windowWidth="18580" windowHeight="12320" tabRatio="500"/>
+    <workbookView xWindow="4875" yWindow="1380" windowWidth="18585" windowHeight="12315" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -487,12 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -518,9 +512,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,6 +520,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,6 +625,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -952,648 +957,648 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="25" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="21" t="s">
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="8" customHeight="1">
+    <row r="3" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="17">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <f>SUM(D4:E6)</f>
         <v>14</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="22">
         <f>A4/7</f>
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <v>3</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="17">
-        <v>2</v>
-      </c>
-      <c r="E5" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5" s="15">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="17">
-        <v>2</v>
-      </c>
-      <c r="E6" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="D6" s="15">
+        <v>2</v>
+      </c>
+      <c r="E6" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="17">
+      <c r="B7" s="6"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <f>SUM(D9:E14)</f>
         <v>23.5</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="22">
         <f>A8/7</f>
         <v>3.3571428571428572</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="15">
         <v>3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="17">
-        <v>2</v>
-      </c>
-      <c r="E10" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="17">
-        <v>2</v>
-      </c>
-      <c r="E11" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11" s="15">
+        <v>2</v>
+      </c>
+      <c r="E11" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="17">
-        <v>2</v>
-      </c>
-      <c r="E13" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="D13" s="15">
+        <v>2</v>
+      </c>
+      <c r="E13" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="17">
-        <v>2</v>
-      </c>
-      <c r="E14" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="D14" s="15">
+        <v>2</v>
+      </c>
+      <c r="E14" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="17">
+      <c r="B15" s="6"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
         <f>SUM(D17:E22)</f>
         <v>23.5</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <f>A16/7</f>
         <v>3.3571428571428572</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="15" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="15">
         <v>3</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="15" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="17">
-        <v>2</v>
-      </c>
-      <c r="E18" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="D18" s="15">
+        <v>2</v>
+      </c>
+      <c r="E18" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="15" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="17">
-        <v>2</v>
-      </c>
-      <c r="E19" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D19" s="15">
+        <v>2</v>
+      </c>
+      <c r="E19" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="15">
         <v>1</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="15" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="17">
-        <v>2</v>
-      </c>
-      <c r="E21" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="D21" s="15">
+        <v>2</v>
+      </c>
+      <c r="E21" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="17">
-        <v>2</v>
-      </c>
-      <c r="E22" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="D22" s="15">
+        <v>2</v>
+      </c>
+      <c r="E22" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="B23" s="6"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="17">
+      <c r="B24" s="6"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
         <f>SUM(D26:E31)</f>
         <v>23.5</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="22">
         <f>A25/7</f>
         <v>3.3571428571428572</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="C25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="15" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="15">
         <v>3</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="15" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="17">
-        <v>2</v>
-      </c>
-      <c r="E27" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="D27" s="15">
+        <v>2</v>
+      </c>
+      <c r="E27" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="15" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="17">
-        <v>2</v>
-      </c>
-      <c r="E28" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="D28" s="15">
+        <v>2</v>
+      </c>
+      <c r="E28" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="15" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="15">
         <v>1</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="15" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="17">
-        <v>2</v>
-      </c>
-      <c r="E30" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="D30" s="15">
+        <v>2</v>
+      </c>
+      <c r="E30" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="15" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="17">
-        <v>2</v>
-      </c>
-      <c r="E31" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="D31" s="15">
+        <v>2</v>
+      </c>
+      <c r="E31" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="18"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="B32" s="6"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="17">
+      <c r="B33" s="6"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
         <f>SUM(D35:E40)</f>
         <v>27.5</v>
       </c>
-      <c r="B34" s="24">
+      <c r="B34" s="22">
         <f>A34/7</f>
         <v>3.9285714285714284</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="18"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="D34" s="15"/>
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="15" t="s">
+      <c r="B35" s="6"/>
+      <c r="C35" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="15">
         <v>3</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="15" t="s">
+      <c r="B36" s="6"/>
+      <c r="C36" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="15">
         <v>3</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="15" t="s">
+      <c r="B37" s="6"/>
+      <c r="C37" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="15">
         <v>3</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="15" t="s">
+      <c r="B38" s="6"/>
+      <c r="C38" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="15">
         <v>1</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="15" t="s">
+      <c r="B39" s="6"/>
+      <c r="C39" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="17">
-        <v>2</v>
-      </c>
-      <c r="E39" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="D39" s="15">
+        <v>2</v>
+      </c>
+      <c r="E39" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="15" t="s">
+      <c r="B40" s="6"/>
+      <c r="C40" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="17">
-        <v>2</v>
-      </c>
-      <c r="E40" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="D40" s="15">
+        <v>2</v>
+      </c>
+      <c r="E40" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="27"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="B41" s="6"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="18"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="17">
+      <c r="B42" s="6"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
         <f>SUM(D44:E48)</f>
         <v>58</v>
       </c>
-      <c r="B43" s="24">
+      <c r="B43" s="22">
         <f>A43/7</f>
         <v>8.2857142857142865</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="18"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="D43" s="15"/>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="15" t="s">
+      <c r="B44" s="6"/>
+      <c r="C44" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="15">
         <v>16</v>
       </c>
-      <c r="E44" s="18"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="E44" s="16"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="15" t="s">
+      <c r="B45" s="6"/>
+      <c r="C45" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18">
+      <c r="D45" s="15"/>
+      <c r="E45" s="16">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="15" t="s">
+      <c r="B46" s="6"/>
+      <c r="C46" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="19">
+      <c r="D46" s="17">
         <v>5</v>
       </c>
-      <c r="E46" s="27">
+      <c r="E46" s="24">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="15" t="s">
+      <c r="B47" s="6"/>
+      <c r="C47" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="17">
-        <v>2</v>
-      </c>
-      <c r="E47" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="D47" s="15">
+        <v>2</v>
+      </c>
+      <c r="E47" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D48" s="17">
-        <v>2</v>
-      </c>
-      <c r="E48" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="D48" s="15">
+        <v>2</v>
+      </c>
+      <c r="E48" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="13"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>38</v>
       </c>
       <c r="B50" s="31"/>
-      <c r="C50" s="12"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="21" t="s">
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="28">
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="25">
         <f>SUM(A4:A50)</f>
         <v>170</v>
       </c>
-      <c r="B52" s="29">
+      <c r="B52" s="26">
         <f>SUM(B4:B50)</f>
         <v>24.285714285714285</v>
       </c>
-      <c r="C52" s="12"/>
+      <c r="C52" s="10"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" ht="9" customHeight="1">
+      <c r="E52" s="7"/>
+    </row>
+    <row r="53" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="12"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="11"/>
+      <c r="E53" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>